<commit_message>
clean-up gpios.h + utils rework
</commit_message>
<xml_diff>
--- a/gpios.xlsx
+++ b/gpios.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\esp32\esp32_common\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC823C86-5D0E-42FB-98E6-872EF1191010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45640271-5589-442B-9D8F-43CFD450D2AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31740" yWindow="2565" windowWidth="21495" windowHeight="12855" activeTab="1" xr2:uid="{08582719-D43F-48F1-8051-6092D0104DDF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{08582719-D43F-48F1-8051-6092D0104DDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$B$2:$F$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$B$4:$F$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="274">
   <si>
     <t>IO1</t>
   </si>
@@ -1144,10 +1145,6 @@
     <t>gate_controller</t>
   </si>
   <si>
-    <t>wp_controller
-WP_HW_V2</t>
-  </si>
-  <si>
     <t>SENSOR_PIN</t>
   </si>
   <si>
@@ -1209,13 +1206,256 @@
   </si>
   <si>
     <t>DS1820</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type </t>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I </t>
+  </si>
+  <si>
+    <t>Module-enable signal. Active high.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SENSOR_VP </t>
+  </si>
+  <si>
+    <t>GPIO36, ADC1_CH0, RTC_GPIO0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SENSOR_VN </t>
+  </si>
+  <si>
+    <t>GPIO39, ADC1_CH3, RTC_GPIO3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO34 </t>
+  </si>
+  <si>
+    <t>GPIO34, ADC1_CH6, RTC_GPIO4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO35 </t>
+  </si>
+  <si>
+    <t>GPIO35, ADC1_CH7, RTC_GPIO5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO32 </t>
+  </si>
+  <si>
+    <t>I/O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO33 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO25 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I/O </t>
+  </si>
+  <si>
+    <t>GPIO25, DAC_1, ADC2_CH8, RTC_GPIO6, EMAC_RXD0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO26 </t>
+  </si>
+  <si>
+    <t>GPIO26, DAC_2, ADC2_CH9, RTC_GPIO7, EMAC_RXD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO27 </t>
+  </si>
+  <si>
+    <t>GPIO27, ADC2_CH7, TOUCH7, RTC_GPIO17, EMAC_RX_DV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHD/SD2* </t>
+  </si>
+  <si>
+    <t>GPIO9, SD_DATA2, SPIHD, HS1_DATA2, U1RXD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWP/SD3* </t>
+  </si>
+  <si>
+    <t>GPIO10, SD_DATA3, SPIWP, HS1_DATA3, U1TXD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCS/CMD* </t>
+  </si>
+  <si>
+    <t>GPIO11, SD_CMD, SPICS0, HS1_CMD, U1RTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCK/CLK* </t>
+  </si>
+  <si>
+    <t>GPIO6, SD_CLK, SPICLK, HS1_CLK, U1CTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDO/SD0* </t>
+  </si>
+  <si>
+    <t>GPIO7, SD_DATA0, SPIQ, HS1_DATA0, U2RTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDI/SD1* </t>
+  </si>
+  <si>
+    <t>GPIO8, SD_DATA1, SPID, HS1_DATA1, U2CTS</t>
+  </si>
+  <si>
+    <t>GPIO0, ADC2_CH1, TOUCH1, RTC_GPIO11, CLK_OUT1, EMAC_TX_CLK</t>
+  </si>
+  <si>
+    <t>GPIO16, HS1_DATA4, U2RXD, EMAC_CLK_OUT</t>
+  </si>
+  <si>
+    <t>GPIO17, HS1_DATA5, U2TXD, EMAC_CLK_OUT_180</t>
+  </si>
+  <si>
+    <t>GPIO5, VSPICS0, HS1_DATA6, EMAC_RX_CLK</t>
+  </si>
+  <si>
+    <t>GPIO18, VSPICLK, HS1_DATA7</t>
+  </si>
+  <si>
+    <t>GPIO19, VSPIQ, U0CTS, EMAC_TXD0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">- </t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>GPIO21, VSPIHD, EMAC_TX_EN</t>
+  </si>
+  <si>
+    <t>GPIO3, U0RXD, CLK_OUT2</t>
+  </si>
+  <si>
+    <t>GPIO1, U0TXD, CLK_OUT3, EMAC_RXD2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO22 </t>
+  </si>
+  <si>
+    <t>GPIO22, VSPIWP, U0RTS, EMAC_TXD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO23 </t>
+  </si>
+  <si>
+    <t>GPIO23, VSPID, HS1_STROBE</t>
+  </si>
+  <si>
+    <t>ESP32-WROOM-32</t>
+  </si>
+  <si>
+    <t>LCD_SCLK</t>
+  </si>
+  <si>
+    <t>LCD_MOSI</t>
+  </si>
+  <si>
+    <t>LCD_DC</t>
+  </si>
+  <si>
+    <t>LCD_RST</t>
+  </si>
+  <si>
+    <t>LCD_CS</t>
+  </si>
+  <si>
+    <t>LCD_BK_LIGHT</t>
+  </si>
+  <si>
+    <t>GPIO4, ADC2_CH0, TOUCH0, RTC_GPIO10, HSPIHD, HS2_DATA1, SD_DATA1, EMAC_TX_ER</t>
+  </si>
+  <si>
+    <t>GPIO2, ADC2_CH2, TOUCH2, RTC_GPIO12, HSPIWP, HS2_DATA0, SD_DATA0</t>
+  </si>
+  <si>
+    <t>GPIO15, ADC2_CH3, TOUCH3, MTDO, HSPICS0, RTC_GPIO13, HS2_CMD, SD_CMD, EMAC_RXD3</t>
+  </si>
+  <si>
+    <t>PIN_NUM_CONVST</t>
+  </si>
+  <si>
+    <t>GPIO14, ADC2_CH6, TOUCH6, RTC_GPIO16, MTMS, HSPICLK, HS2_CLK, SD_CLK, EMAC_TXD2</t>
+  </si>
+  <si>
+    <t>GPIO12, ADC2_CH5, TOUCH5, RTC_GPIO15, MTDI, HSPIQ, HS2_DATA2, SD_DATA2, EMAC_TXD3</t>
+  </si>
+  <si>
+    <t>PIN_NUM_QMETER</t>
+  </si>
+  <si>
+    <t>PIN_NUM_MISO</t>
+  </si>
+  <si>
+    <t>PIN_NUM_MOSI</t>
+  </si>
+  <si>
+    <t>PIN_NUM_CLK</t>
+  </si>
+  <si>
+    <t>ROT_ENC_S1</t>
+  </si>
+  <si>
+    <t>ROT_ENC_S2</t>
+  </si>
+  <si>
+    <t>GPIO32, XTAL_32K_P (32.768 kHz crystal oscillator input), ADC1_CH4, TOUCH9, RTC_GPIO9</t>
+  </si>
+  <si>
+    <t>GPIO33, XTAL_32K_N (32.768 kHz crystal oscillator output), ADC1_CH5, TOUCH8, RTC_GPIO8</t>
+  </si>
+  <si>
+    <t>ROT_ENC_KEY</t>
+  </si>
+  <si>
+    <t>GPIO13, ADC2_CH4, TOUCH4, RTC_GPIO14, MTCK, HSPID, HS2_DATA3, SD_DATA3, EMAC_RX_ER</t>
+  </si>
+  <si>
+    <t>PINEN_DV2</t>
+  </si>
+  <si>
+    <t>PINEN_DV3</t>
+  </si>
+  <si>
+    <t>WP_CONTROLLER</t>
+  </si>
+  <si>
+    <t>HW_V1</t>
+  </si>
+  <si>
+    <t>HW_V2</t>
+  </si>
+  <si>
+    <t>Pins available in HW v1 &amp; v2</t>
+  </si>
+  <si>
+    <t>Pins available in HW v2 only</t>
+  </si>
+  <si>
+    <t>V1 &amp; V2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1249,8 +1489,19 @@
       <color rgb="FF000000"/>
       <name val="HelveticaNeue-Medium-Identity-H"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1263,8 +1514,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1296,11 +1571,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1308,20 +1592,47 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1339,6 +1650,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>140500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>116679</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>507941</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>152398</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CF8EA49-44BA-4FFE-A462-4728DD3CB969}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="11583961" y="3208368"/>
+          <a:ext cx="3274219" cy="2805841"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>771525</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>159578</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1D74F6B-F07C-5740-F2E6-A516667CB5D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8324850" y="3267076"/>
+          <a:ext cx="3067050" cy="3369502"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1660,7 +2064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{294AEDC3-1A68-40A4-9DFD-88938BF51E96}">
   <dimension ref="B2:B81"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2074,10 +2478,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F812EE-6D19-42CA-9916-D91804553614}">
-  <dimension ref="A1:K43"/>
+  <dimension ref="B1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2087,819 +2491,1576 @@
     <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="70.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" customWidth="1"/>
     <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30">
-      <c r="A1" s="5"/>
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="2:10">
+      <c r="B1" s="4"/>
+      <c r="C1" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+    </row>
+    <row r="2" spans="2:10">
+      <c r="B2" s="16"/>
+      <c r="C2" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+    </row>
+    <row r="3" spans="2:10">
+      <c r="B3" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="G1" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="G3" t="s">
         <v>169</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I3" t="s">
+        <v>170</v>
+      </c>
+      <c r="J3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="B4" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="4">
+        <v>27</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="4">
+        <v>39</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>175</v>
+      </c>
+      <c r="I6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="20">
+        <v>38</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="4">
+        <v>15</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>177</v>
+      </c>
+      <c r="H8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="4">
+        <v>4</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>173</v>
+      </c>
+      <c r="H9" t="s">
+        <v>184</v>
+      </c>
+      <c r="I9" t="s">
+        <v>186</v>
+      </c>
+      <c r="J9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="4">
+        <v>5</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>172</v>
+      </c>
+      <c r="I10" t="s">
+        <v>185</v>
+      </c>
+      <c r="J10" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="4">
+        <v>6</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+      <c r="G11" t="s">
+        <v>174</v>
+      </c>
+      <c r="H11" t="s">
         <v>180</v>
       </c>
-      <c r="I1" t="s">
-        <v>170</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="K1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="B2" s="2" t="s">
+      <c r="I11" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="4">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12">
+        <v>7</v>
+      </c>
+      <c r="G12" t="s">
+        <v>178</v>
+      </c>
+      <c r="H12" t="s">
+        <v>181</v>
+      </c>
+      <c r="I12" t="s">
+        <v>188</v>
+      </c>
+      <c r="J12" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="4">
+        <v>12</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13">
+        <v>8</v>
+      </c>
+      <c r="G13" t="s">
+        <v>176</v>
+      </c>
+      <c r="H13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="4">
+        <v>17</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="4">
+        <v>18</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="4">
+        <v>19</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" s="4">
+        <v>20</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="20">
+        <v>21</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="F18">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="1">
+        <v>22</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="20">
+        <v>8</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="20">
+        <v>9</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="20">
+        <v>10</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="20">
+        <v>11</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="4">
+        <v>13</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F24">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="4">
+        <v>14</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="1">
+        <v>23</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F26">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C27" s="20">
+        <v>28</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="F27">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="20">
+        <v>29</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F28">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="B29" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="C29" s="20">
+        <v>30</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="F29">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="B30" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" s="20">
+        <v>31</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="F30">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="C31" s="20">
+        <v>32</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="F31">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="B32" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="C32" s="20">
+        <v>33</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="F32">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="C33" s="20">
+        <v>34</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="F33">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="C34" s="20">
+        <v>35</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="F34">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" s="4">
+        <v>37</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="B36" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C36" s="4">
+        <v>36</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F36">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="B37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" s="1">
+        <v>26</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F37">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="B38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="1">
+        <v>16</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F38">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="B39" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" s="1">
+        <v>24</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F39">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="B40" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" s="1">
+        <v>25</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F40">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="B41" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C41" s="1">
+        <v>41</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F41" s="3" t="str">
+        <f>MID(B41, 3, 2)</f>
+        <v>AD</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="B42" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C42" s="1">
+        <v>40</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F42" s="3" t="str">
+        <f>MID(B42, 3, 2)</f>
+        <v xml:space="preserve">D </v>
+      </c>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="B43" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="B44" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C44" s="1">
+        <v>2</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" ht="38.25">
+      <c r="B45" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C45" s="4">
+        <v>3</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B4:F4" xr:uid="{D3F812EE-6D19-42CA-9916-D91804553614}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:F45">
+      <sortCondition ref="F4"/>
+    </sortState>
+  </autoFilter>
+  <mergeCells count="3">
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02CCD2D6-93C4-496C-B515-DF91BF3E886B}">
+  <dimension ref="B1:G42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="90.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7">
+      <c r="F1" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="2:7">
+      <c r="F2" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="G3" s="19"/>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D4" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="B3" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C3" s="1">
-        <v>27</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="B4" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C4" s="7">
-        <v>39</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="F4">
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="G4" t="s">
-        <v>176</v>
-      </c>
-      <c r="I4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="B5" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C5" s="1">
-        <v>38</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>81</v>
+        <v>155</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F5">
+        <v>194</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="B6" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="7">
-        <v>15</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="F6">
+      <c r="D6" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" s="1">
         <v>3</v>
       </c>
-      <c r="G6" t="s">
-        <v>178</v>
-      </c>
-      <c r="H6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="B7" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7" s="7">
+      <c r="D7" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C8" s="1">
         <v>4</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F7">
-        <v>4</v>
-      </c>
-      <c r="G7" t="s">
-        <v>174</v>
-      </c>
-      <c r="H7" t="s">
-        <v>185</v>
-      </c>
-      <c r="I7" t="s">
-        <v>187</v>
-      </c>
-      <c r="K7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="B8" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="7">
+      <c r="D8" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="11" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9" s="1">
         <v>5</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F8">
-        <v>5</v>
-      </c>
-      <c r="G8" t="s">
-        <v>173</v>
-      </c>
-      <c r="I8" t="s">
-        <v>186</v>
-      </c>
-      <c r="K8" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="B9" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C9" s="7">
+      <c r="D9" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" s="1">
         <v>6</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F9">
-        <v>6</v>
-      </c>
-      <c r="G9" t="s">
-        <v>175</v>
-      </c>
-      <c r="H9" t="s">
-        <v>181</v>
-      </c>
-      <c r="I9" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="B10" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" s="7">
+      <c r="D10" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C11" s="1">
         <v>7</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="F10">
-        <v>7</v>
-      </c>
-      <c r="G10" t="s">
-        <v>179</v>
-      </c>
-      <c r="H10" t="s">
-        <v>182</v>
-      </c>
-      <c r="I10" t="s">
-        <v>189</v>
-      </c>
-      <c r="K10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="B11" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C11" s="7">
+      <c r="D11" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C12" s="1">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C13" s="1">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C14" s="1">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C15" s="1">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C16" s="1">
         <v>12</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F11">
-        <v>8</v>
-      </c>
-      <c r="G11" t="s">
-        <v>177</v>
-      </c>
-      <c r="H11" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="B12" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C12" s="7">
-        <v>17</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="F12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="B13" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" s="7">
-        <v>18</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="F13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="B14" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C14" s="7">
-        <v>19</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F14">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="B15" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C15" s="7">
-        <v>20</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="F15">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="B16" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C16" s="1">
-        <v>21</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>110</v>
+        <v>209</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F16">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6">
+        <v>214</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="2:7">
       <c r="B17" s="1" t="s">
         <v>114</v>
       </c>
       <c r="C17" s="1">
+        <v>13</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" s="1">
+        <v>14</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C19" s="1">
+        <v>15</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="1">
+        <v>16</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="11" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C21" s="1">
+        <v>17</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C22" s="1">
+        <v>18</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C23" s="1">
+        <v>19</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C24" s="1">
+        <v>20</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C25" s="1">
+        <v>21</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C26" s="1">
         <v>22</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F17">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6">
-      <c r="B18" s="1" t="s">
+      <c r="D26" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C18" s="1">
-        <v>8</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F18">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6">
-      <c r="B19" s="1" t="s">
+      <c r="C27" s="1">
+        <v>23</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" s="1">
+        <v>24</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="1">
+        <v>25</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="1">
+        <v>26</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="B31" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="1">
-        <v>9</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F19">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6">
-      <c r="B20" s="1" t="s">
+      <c r="C31" s="1">
+        <v>27</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="B32" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="1">
-        <v>10</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F20">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6">
-      <c r="B21" s="1" t="s">
+      <c r="C32" s="1">
+        <v>28</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="G32" s="18"/>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="1">
+        <v>29</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="G33" s="18"/>
+    </row>
+    <row r="34" spans="2:7">
+      <c r="B34" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="1">
-        <v>11</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F21">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6">
-      <c r="B22" s="1" t="s">
+      <c r="C34" s="1">
+        <v>30</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="G34" s="18"/>
+    </row>
+    <row r="35" spans="2:7">
+      <c r="B35" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="1">
-        <v>13</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F22">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6">
-      <c r="B23" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23" s="1">
-        <v>14</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F23">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6">
-      <c r="B24" s="1" t="s">
+      <c r="C35" s="1">
+        <v>31</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="G35" s="18"/>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="B36" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C36" s="1">
+        <v>32</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C24" s="1">
-        <v>23</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F24">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6">
-      <c r="B25" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C25" s="1">
-        <v>28</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F25">
+      <c r="C37" s="1">
+        <v>33</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="G37" s="18"/>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C38" s="1">
+        <v>34</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="B39" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C39" s="1">
         <v>35</v>
       </c>
-    </row>
-    <row r="26" spans="2:6">
-      <c r="B26" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C26" s="1">
-        <v>29</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F26">
+      <c r="D39" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+    </row>
+    <row r="40" spans="2:7">
+      <c r="B40" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C40" s="1">
         <v>36</v>
       </c>
-    </row>
-    <row r="27" spans="2:6">
-      <c r="B27" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C27" s="1">
-        <v>30</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F27">
+      <c r="D40" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="G40" s="18"/>
+    </row>
+    <row r="41" spans="2:7">
+      <c r="B41" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C41" s="1">
         <v>37</v>
       </c>
-    </row>
-    <row r="28" spans="2:6">
-      <c r="B28" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C28" s="1">
-        <v>31</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="F28">
+      <c r="D41" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7">
+      <c r="B42" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C42" s="1">
         <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6">
-      <c r="B29" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C29" s="1">
-        <v>32</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F29">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6">
-      <c r="B30" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C30" s="1">
-        <v>33</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="F30">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6">
-      <c r="B31" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C31" s="1">
-        <v>34</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="F31">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6">
-      <c r="B32" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C32" s="1">
-        <v>35</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F32">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6">
-      <c r="B33" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="C33" s="7">
-        <v>37</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="F33">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6">
-      <c r="B34" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C34" s="7">
-        <v>36</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="F34">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6">
-      <c r="B35" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C35" s="1">
-        <v>26</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F35">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6">
-      <c r="B36" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C36" s="1">
-        <v>16</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F36">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6">
-      <c r="B37" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C37" s="1">
-        <v>24</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F37">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6">
-      <c r="B38" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C38" s="1">
-        <v>25</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F38">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6">
-      <c r="B39" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C39" s="1">
-        <v>41</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F39" s="4" t="str">
-        <f>MID(B39, 3, 2)</f>
-        <v>AD</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6">
-      <c r="B40" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C40" s="1">
-        <v>40</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F40" s="4" t="str">
-        <f>MID(B40, 3, 2)</f>
-        <v xml:space="preserve">D </v>
-      </c>
-    </row>
-    <row r="41" spans="2:6">
-      <c r="B41" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C41" s="1">
-        <v>1</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6">
-      <c r="B42" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C42" s="1">
-        <v>2</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>155</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" ht="38.25">
-      <c r="B43" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C43" s="1">
-        <v>3</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>163</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:F2" xr:uid="{D3F812EE-6D19-42CA-9916-D91804553614}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:F43">
-      <sortCondition ref="F2"/>
-    </sortState>
-  </autoFilter>
-  <mergeCells count="1">
-    <mergeCell ref="B1:E1"/>
+  <mergeCells count="9">
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F37:G37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>